<commit_message>
strategy pattern implementation, minor changes in conditions
</commit_message>
<xml_diff>
--- a/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample90-file.xlsx
+++ b/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample90-file.xlsx
@@ -376,8 +376,8 @@
     <cellStyle name="WCSecondStyle_Alternate" xfId="23"/>
     <cellStyle name="QuantityEqualsToConditionStyle" xfId="24"/>
     <cellStyle name="QuantityEqualsToConditionStyle_Alternate" xfId="25"/>
-    <cellStyle name="PriceyEqualsToConditionStyle" xfId="26"/>
-    <cellStyle name="PriceyEqualsToConditionStyle_Alternate" xfId="27"/>
+    <cellStyle name="RemarksProductStyle" xfId="26"/>
+    <cellStyle name="RemarksProductStyle_Alternate" xfId="27"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
@@ -409,121 +409,121 @@
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="10">
         <v>37</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="6">
         <v>3.9900000095367432</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="6">
         <v>147.6300048828125</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="11">
         <v>5</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="7">
         <v>12.100000381469727</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="7">
         <v>60.5</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="10">
         <v>7</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="6">
         <v>22.100000381469727</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="6">
         <v>100.5</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="11">
         <v>12</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="7">
         <v>15.369999885559082</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="7">
         <v>184.44000244140625</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="10">
         <v>20</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="6">
         <v>8</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="6">
         <v>160</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="11">
         <v>7</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="7">
         <v>23.479999542236328</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="7">
         <v>164.36000061035156</v>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="20">
+      <c r="C9" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="10">
         <v>7</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="6">
         <v>22.100000381469727</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="6">
         <v>100.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
patterns and initial support filterdata
</commit_message>
<xml_diff>
--- a/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample90-file.xlsx
+++ b/source/samples/export/iTin.Export.Queries.SqlServerCeSample/output/sample9x/fromconfigfile/sample90-file.xlsx
@@ -9,7 +9,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'EPPlus - Some data'!$B$2:$F$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'EPPlus - Some data'!$A$1:$F$11</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'EPPlus - Some data'!$A$1:$F$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'EPPlus - Some data'!$1:$2</definedName>
   </definedNames>
   <calcPr fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Id</t>
   </si>
@@ -34,34 +34,10 @@
     <t>Value</t>
   </si>
   <si>
-    <t>12001</t>
-  </si>
-  <si>
-    <t>Nails</t>
-  </si>
-  <si>
     <t>12002</t>
   </si>
   <si>
     <t>Hammer</t>
-  </si>
-  <si>
-    <t>12003</t>
-  </si>
-  <si>
-    <t>Saw</t>
-  </si>
-  <si>
-    <t>12010</t>
-  </si>
-  <si>
-    <t>Drill</t>
-  </si>
-  <si>
-    <t>12013</t>
-  </si>
-  <si>
-    <t>Crowbar</t>
   </si>
 </sst>
 </file>
@@ -385,7 +361,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2:F10"/>
+  <dimension ref="B2:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="1"/>
   </sheetViews>
@@ -416,128 +392,43 @@
         <v>6</v>
       </c>
       <c r="D3" s="10">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="E3" s="6">
-        <v>3.9900000095367432</v>
+        <v>12.100000381469727</v>
       </c>
       <c r="F3" s="6">
-        <v>147.6300048828125</v>
+        <v>60.5</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="11">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="11">
-        <v>5</v>
-      </c>
       <c r="E4" s="7">
-        <v>12.100000381469727</v>
+        <v>22.100000381469727</v>
       </c>
       <c r="F4" s="7">
-        <v>60.5</v>
+        <v>100.5</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="10">
-        <v>7</v>
-      </c>
-      <c r="E5" s="6">
-        <v>22.100000381469727</v>
-      </c>
-      <c r="F5" s="6">
-        <v>100.5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="11">
-        <v>12</v>
-      </c>
-      <c r="E6" s="7">
-        <v>15.369999885559082</v>
-      </c>
-      <c r="F6" s="7">
-        <v>184.44000244140625</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="10">
-        <v>20</v>
-      </c>
-      <c r="E7" s="6">
-        <v>8</v>
-      </c>
-      <c r="F7" s="6">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="11">
-        <v>7</v>
-      </c>
-      <c r="E8" s="7">
-        <v>23.479999542236328</v>
-      </c>
-      <c r="F8" s="7">
-        <v>164.36000061035156</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="10">
-        <v>7</v>
-      </c>
-      <c r="E9" s="6">
-        <v>22.100000381469727</v>
-      </c>
-      <c r="F9" s="6">
-        <v>100.5</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12">
-        <f>SUBTOTAL(109,D3:D9)</f>
-      </c>
-      <c r="E10" s="8">
-        <f>SUBTOTAL(109,E3:E9)</f>
-      </c>
-      <c r="F10" s="8">
-        <f>SUBTOTAL(109,F3:F9)</f>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12">
+        <f>SUBTOTAL(109,D3:D4)</f>
+      </c>
+      <c r="E5" s="8">
+        <f>SUBTOTAL(109,E3:E4)</f>
+      </c>
+      <c r="F5" s="8">
+        <f>SUBTOTAL(109,F3:F4)</f>
       </c>
     </row>
   </sheetData>

</xml_diff>